<commit_message>
Update template file in
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF006_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF006_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02.Project\UK\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UKworkspace2\nts.uk\uk.at\at.ctx\request\nts.uk.ctx.at.request.infra\src\main\resources\application\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -422,50 +422,50 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -515,7 +515,7 @@
         <xdr:cNvPr id="2" name="APPORVAL1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B1955F-FA3E-45BD-8AA6-7885D40B32DC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -534,7 +534,7 @@
           <xdr:cNvPr id="3" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C156E10C-E8B7-4F45-BD6D-D2978AA38071}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -588,7 +588,7 @@
           <xdr:cNvPr id="4" name="直線コネクタ 3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79C99138-C43F-404A-A5C2-88915EFFD6CB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -628,7 +628,7 @@
           <xdr:cNvPr id="5" name="直線コネクタ 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{721F4046-D62E-424A-A00A-B8D6D3BCC753}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -668,7 +668,7 @@
           <xdr:cNvPr id="6" name="NAME1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C792741C-68A4-46BA-82E7-1845939D95C4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -710,8 +710,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -721,7 +721,7 @@
           <xdr:cNvPr id="7" name="STATUS1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{557EB40E-E6F5-4E5C-B2FE-2480DEEBBC0E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -763,8 +763,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -774,7 +774,7 @@
           <xdr:cNvPr id="8" name="DATE1">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1674D596-31FB-4C98-B939-B6D0C035E2D6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -816,8 +816,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -843,7 +843,7 @@
         <xdr:cNvPr id="9" name="APPORVAL2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F06F0980-4862-4824-9E5F-2A5770158EDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -862,7 +862,7 @@
           <xdr:cNvPr id="10" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587707DB-109D-46B4-8C8F-73469D36B9CA}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -916,7 +916,7 @@
           <xdr:cNvPr id="11" name="直線コネクタ 10">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AD2029F-4454-473F-8CFA-DF2216C7E806}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -956,7 +956,7 @@
           <xdr:cNvPr id="12" name="直線コネクタ 11">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0DC3E96-3055-489A-B89B-9C9DA194D093}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -996,7 +996,7 @@
           <xdr:cNvPr id="13" name="NAME2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D81417FD-0A6E-44E8-B0CB-497AEAA9CEF6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1059,7 +1059,7 @@
           <xdr:cNvPr id="14" name="STATUS2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C49E7F4-02AD-47BB-A967-EDA5D8BAA02C}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1101,8 +1101,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1112,7 +1112,7 @@
           <xdr:cNvPr id="15" name="DATE2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8389EC5-0245-4ABC-B1B7-22F833B11C11}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1154,8 +1154,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1181,7 +1181,7 @@
         <xdr:cNvPr id="16" name="APPORVAL3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B0489C8-56BF-4F73-A0C2-115614ACDC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1200,7 +1200,7 @@
           <xdr:cNvPr id="17" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59FC0746-AEEC-4C26-AF80-BF981A6F5DAC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1254,7 +1254,7 @@
           <xdr:cNvPr id="18" name="直線コネクタ 17">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1242A7C-8301-47B5-B8ED-8C3D706BD351}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1294,7 +1294,7 @@
           <xdr:cNvPr id="19" name="直線コネクタ 18">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF27655A-17E2-480E-983E-58A3E4F4D9D9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1334,7 +1334,7 @@
           <xdr:cNvPr id="20" name="NAME3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DA712EC-A8B9-4EFA-8339-034A61062227}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1376,8 +1376,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1387,7 +1387,7 @@
           <xdr:cNvPr id="21" name="STATUS3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3462ABC4-A7E5-4EB8-A86C-6C960B6BFBD1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1429,8 +1429,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1440,7 +1440,7 @@
           <xdr:cNvPr id="22" name="DATE3">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89DF5A57-EC28-4737-ACB5-FCCFC1EFD4FC}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1482,8 +1482,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1509,7 +1509,7 @@
         <xdr:cNvPr id="23" name="APPORVAL4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0BC8B37-9CEF-4D59-B05E-C508415DB387}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1528,7 +1528,7 @@
           <xdr:cNvPr id="24" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73105E46-4471-451B-8EF7-129886A0AE58}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1582,7 +1582,7 @@
           <xdr:cNvPr id="25" name="直線コネクタ 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECC25DB-00F4-493A-9BDE-192A731F2FA1}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1622,7 +1622,7 @@
           <xdr:cNvPr id="26" name="直線コネクタ 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{924C7365-89A6-4173-90F9-6FC918BF4051}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1662,7 +1662,7 @@
           <xdr:cNvPr id="27" name="NAME4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A13E55-AAE5-48D3-93F0-9A79E2876E6F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1704,8 +1704,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1715,7 +1715,7 @@
           <xdr:cNvPr id="28" name="STATUS4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3C2753F-2565-428D-AADC-9DA451DCA14B}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1757,8 +1757,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1768,7 +1768,7 @@
           <xdr:cNvPr id="29" name="DATE4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9862509B-BF03-4C2C-9AFC-89B1668E70E2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1810,8 +1810,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1837,7 +1837,7 @@
         <xdr:cNvPr id="30" name="APPORVAL5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AC3BCDD-453E-4168-97E5-6465C768C0C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1856,7 +1856,7 @@
           <xdr:cNvPr id="31" name="円/楕円 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16E93C03-999C-41C9-9E66-42EBB20BE593}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1910,7 +1910,7 @@
           <xdr:cNvPr id="32" name="直線コネクタ 31">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0616920-9A62-4D8B-87E3-1DE272A793DF}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1950,7 +1950,7 @@
           <xdr:cNvPr id="33" name="直線コネクタ 32">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2C26E7-0AEF-4870-8CD1-5479D5CF6061}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1990,7 +1990,7 @@
           <xdr:cNvPr id="34" name="NAME5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53B74D66-215D-4DB5-9861-3EE95021CB6E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2032,8 +2032,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -2043,7 +2043,7 @@
           <xdr:cNvPr id="35" name="STATUS5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63EBCD51-4BD6-4130-9F29-5BC13BB46EDB}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2085,8 +2085,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -2096,7 +2096,7 @@
           <xdr:cNvPr id="36" name="DATE5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E139FF7-9B45-4F04-9E76-61C46585964F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2138,8 +2138,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -2573,10 +2573,10 @@
     <row r="3" spans="1:12" ht="15" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="27"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
@@ -2587,10 +2587,10 @@
     <row r="4" spans="1:12" ht="15" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="27"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -2614,142 +2614,142 @@
     </row>
     <row r="6" spans="1:12" ht="30" customHeight="1">
       <c r="A6" s="1"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="34"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="40"/>
       <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" ht="30" customHeight="1">
       <c r="A7" s="1"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="34"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="40"/>
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1">
       <c r="A8" s="1"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="34"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="40"/>
       <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:12" ht="30" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="34"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="40"/>
       <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="34"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="40"/>
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="1"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="34"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="40"/>
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="28"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="34"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="40"/>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="34"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="40"/>
       <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="34"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="40"/>
       <c r="L14" s="1"/>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="32"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="34"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="40"/>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="3.75" customHeight="1">
@@ -2768,16 +2768,16 @@
     </row>
     <row r="17" spans="1:12" ht="90" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
-      <c r="K17" s="39"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="32"/>
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="3.75" customHeight="1">
@@ -2810,16 +2810,16 @@
     </row>
     <row r="20" spans="1:12" ht="74.25" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="42"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="35"/>
       <c r="L20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="3.75" customHeight="1">
@@ -3029,16 +3029,6 @@
     <row r="44" spans="2:11" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:K20"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D13:K13"/>
-    <mergeCell ref="D14:K14"/>
-    <mergeCell ref="D15:K15"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="C4:F4"/>
@@ -3055,6 +3045,16 @@
     <mergeCell ref="D10:K10"/>
     <mergeCell ref="D11:K11"/>
     <mergeCell ref="D12:K12"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:K20"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D13:K13"/>
+    <mergeCell ref="D14:K14"/>
+    <mergeCell ref="D15:K15"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Update template font chu
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF006_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/request/nts.uk.ctx.at.request.infra/src/main/resources/application/KAF006_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="休暇申請" sheetId="29" r:id="rId1"/>
@@ -53,7 +53,6 @@
     <definedName name="kkkk" hidden="1">#REF!</definedName>
     <definedName name="ｌ" localSheetId="0" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
     <definedName name="ｌ" hidden="1">{"VIEW1",#N/A,FALSE,"春木";"VIEW2",#N/A,FALSE,"春木";"VIEW3",#N/A,FALSE,"春木"}</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">休暇申請!$A$1:$L$29</definedName>
     <definedName name="sss" hidden="1">#REF!</definedName>
     <definedName name="Ver002001006特休残管理対応" hidden="1">#REF!</definedName>
     <definedName name="wrn.MIND." localSheetId="0" hidden="1">{#N/A,#N/A,TRUE,"Sheet2";#N/A,#N/A,TRUE,"Sheet3";#N/A,#N/A,TRUE,"Sheet4";#N/A,#N/A,TRUE,"Sheet1"}</definedName>
@@ -710,8 +709,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -763,8 +762,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -816,8 +815,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1034,16 +1033,6 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-                <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900">
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
@@ -1101,8 +1090,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1154,8 +1143,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1376,8 +1365,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1429,8 +1418,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1482,8 +1471,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1704,8 +1693,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1757,8 +1746,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -1810,8 +1799,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -2032,8 +2021,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -2085,8 +2074,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>
@@ -2138,8 +2127,8 @@
               <a:solidFill>
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
-              <a:latin typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
-              <a:ea typeface="ＭＳ 明朝" panose="02020609040205080304" pitchFamily="17" charset="-128"/>
+              <a:latin typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="源ノ角ゴシック JP Normal" panose="020B0400000000000000" pitchFamily="34" charset="-128"/>
             </a:endParaRPr>
           </a:p>
         </xdr:txBody>

</xml_diff>